<commit_message>
further developed the web parsing aspect
</commit_message>
<xml_diff>
--- a/combinations.xlsx
+++ b/combinations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="73">
   <si>
     <t>LUNES</t>
   </si>
@@ -218,10 +218,24 @@
     <t>22:00</t>
   </si>
   <si>
-    <t xml:space="preserve"> Psicología Educacional  1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Psicología Educacional  2</t>
+    <t>22:15</t>
+  </si>
+  <si>
+    <t>22:30</t>
+  </si>
+  <si>
+    <t>22:45</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teoría y Técnica de Exploración 
+y Diagnóstico Psicológico Módulo I  3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teoría y Técnica de Exploración 
+y Diagnóstico Psicológico Módulo I  8</t>
   </si>
 </sst>
 </file>
@@ -260,13 +274,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1F77B4"/>
+        <fgColor rgb="FF2CA02C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF17BECF"/>
+        <fgColor rgb="FF1F77B4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,13 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" customWidth="1"/>
@@ -1138,7 +1152,7 @@
         <v>50</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1151,7 +1165,7 @@
         <v>51</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1164,7 +1178,7 @@
         <v>52</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1177,7 +1191,7 @@
         <v>53</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -1190,7 +1204,7 @@
         <v>54</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1203,7 +1217,7 @@
         <v>55</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -1227,7 +1241,7 @@
         <v>57</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1240,7 +1254,7 @@
         <v>58</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -1253,7 +1267,7 @@
         <v>59</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -1266,7 +1280,7 @@
         <v>60</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1279,7 +1293,7 @@
         <v>61</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -1292,7 +1306,7 @@
         <v>62</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -1305,7 +1319,7 @@
         <v>63</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -1318,7 +1332,7 @@
         <v>64</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1331,7 +1345,7 @@
         <v>65</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -1343,12 +1357,64 @@
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1357,17 +1423,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1421,9 +1487,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7">
@@ -1434,9 +1498,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
@@ -1447,9 +1509,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7">
@@ -1460,9 +1520,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7">
@@ -1473,9 +1531,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7">
@@ -1486,9 +1542,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7">
@@ -1499,9 +1553,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7">
@@ -1512,9 +1564,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7">
@@ -1525,9 +1575,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
@@ -1538,9 +1586,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
@@ -1551,9 +1597,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
@@ -1564,9 +1608,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
@@ -1577,9 +1619,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
@@ -1601,9 +1641,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7">
@@ -1614,9 +1652,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7">
@@ -1627,9 +1663,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7">
@@ -1640,9 +1674,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7">
@@ -1653,9 +1685,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7">
@@ -1666,9 +1696,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7">
@@ -1917,7 +1945,9 @@
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1928,7 +1958,9 @@
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1939,7 +1971,9 @@
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1950,7 +1984,9 @@
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1961,7 +1997,9 @@
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1972,7 +2010,9 @@
       <c r="A51" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1994,7 +2034,9 @@
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2005,7 +2047,9 @@
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2016,7 +2060,9 @@
       <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2027,7 +2073,9 @@
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2038,7 +2086,9 @@
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2049,7 +2099,9 @@
       <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -2060,7 +2112,9 @@
       <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -2071,7 +2125,9 @@
       <c r="A60" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -2082,7 +2138,9 @@
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -2093,13 +2151,65 @@
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="2"/>
+      <c r="B62" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>